<commit_message>
Next Version Dev - collate removed - added test Article (FileTypes) - added expore_it and other functions - read_it, read_tables (concept finalized) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/read_it.xlsx
+++ b/00_nightly_only/read_it.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>read it behaviour</t>
   </si>
@@ -165,6 +165,57 @@
   </si>
   <si>
     <t>Table_Field / cell-df</t>
+  </si>
+  <si>
+    <t>value_attribute_classify</t>
+  </si>
+  <si>
+    <t>Table_Field / cell-df (with VA classification)</t>
+  </si>
+  <si>
+    <t>cell_analysis</t>
+  </si>
+  <si>
+    <t>analyze_cells / analyse_cells</t>
+  </si>
+  <si>
+    <t>basic_classifier</t>
+  </si>
+  <si>
+    <t>numeric_values_classifier</t>
+  </si>
+  <si>
+    <t>sample_based_classifier</t>
+  </si>
+  <si>
+    <t>general VA classifier (which takes VA classification function as input)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number like cells are considered as values and rest as atribute. </t>
+  </si>
+  <si>
+    <t>basic VA classifier which consider numeric (already numeric) as values and text as attribute</t>
+  </si>
+  <si>
+    <t>sample based VA classifier where connected cells are marked same as the match.</t>
+  </si>
+  <si>
+    <t>complete heuristic based structure allocation</t>
+  </si>
+  <si>
+    <t>compose_cells</t>
+  </si>
+  <si>
+    <t>tibble</t>
+  </si>
+  <si>
+    <t>tidy form (without datablock wise column collation)</t>
+  </si>
+  <si>
+    <t>compose_cells(discard_raw_cols = TRUE)</t>
+  </si>
+  <si>
+    <t>tidy form (without datablock wise column collation) (ideal if data-block wise variation is not present)</t>
   </si>
 </sst>
 </file>
@@ -532,19 +583,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -851,21 +902,99 @@
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>